<commit_message>
Actualización del archivo Encuesta.xlsx
</commit_message>
<xml_diff>
--- a/Encuesta.xlsx
+++ b/Encuesta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benja\OneDrive\Escritorio\Prueba Visualización Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BCBA443-6476-4FB4-BB75-6635FFA6418F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4EAE3A-09DD-4DE4-AEC4-43FED4E66465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -126,26 +126,6 @@
     <t>Marca temporal</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Pregunta Abierta (Opcional):</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">
- Basándote en tu experiencia, ¿Qué sugerencias tienes para mejorar la formación académica en el área de la computación?</t>
-    </r>
-  </si>
-  <si>
     <t>Java</t>
   </si>
   <si>
@@ -311,6 +291,9 @@
   </si>
   <si>
     <t>Metodologías Ágiles</t>
+  </si>
+  <si>
+    <t>Pregunta Abierta</t>
   </si>
 </sst>
 </file>
@@ -320,7 +303,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -358,6 +341,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -379,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -392,6 +382,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -612,9 +603,9 @@
   </sheetPr>
   <dimension ref="A1:AW26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AH23" sqref="AH23"/>
+      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -622,153 +613,153 @@
     <col min="1" max="55" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:49" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="4" t="s">
+      <c r="O1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="AA1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AD1" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="AE1" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH1" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AK1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AL1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AK1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AQ1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AR1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AP1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AS1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AU1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="AR1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AV1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AW1" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="AU1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="AV1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:49" x14ac:dyDescent="0.2">
@@ -946,7 +937,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K3" s="1">
         <v>5</v>
@@ -1095,7 +1086,7 @@
         <v>2</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K4" s="1">
         <v>3</v>
@@ -1536,7 +1527,7 @@
         <v>2</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K7" s="1">
         <v>4</v>
@@ -1831,7 +1822,7 @@
         <v>4</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K9" s="1">
         <v>4</v>
@@ -2126,7 +2117,7 @@
         <v>1</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K11" s="1">
         <v>3</v>
@@ -2567,7 +2558,7 @@
         <v>4</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K14" s="1">
         <v>4</v>
@@ -3446,7 +3437,7 @@
         <v>1</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K20" s="1">
         <v>4</v>
@@ -3566,7 +3557,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:49" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>45547.657087627318</v>
       </c>
@@ -3595,7 +3586,7 @@
         <v>2</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K21" s="1">
         <v>4</v>
@@ -4299,7 +4290,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:49" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>45550.828875115738</v>
       </c>

</xml_diff>

<commit_message>
Pequeña actualización, pruebas agregando html y css.
</commit_message>
<xml_diff>
--- a/Encuesta.xlsx
+++ b/Encuesta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benja\OneDrive\Escritorio\Prueba Visualización Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4EAE3A-09DD-4DE4-AEC4-43FED4E66465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67779944-00D7-4050-98B3-D76845B35A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Marca temporal</t>
   </si>
@@ -294,6 +294,9 @@
   </si>
   <si>
     <t>Pregunta Abierta</t>
+  </si>
+  <si>
+    <t>Más ramos de desarrollo web al principio de la carrera</t>
   </si>
 </sst>
 </file>
@@ -369,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -383,6 +386,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -601,11 +606,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AW26"/>
+  <dimension ref="A1:AW27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
+      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -762,7 +767,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:49" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>45540.672958310184</v>
       </c>
@@ -908,7 +913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:49" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>45540.675037175926</v>
       </c>
@@ -1057,7 +1062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:49" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>45540.693168807869</v>
       </c>
@@ -1206,7 +1211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:49" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>45540.693871539348</v>
       </c>
@@ -1352,7 +1357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:49" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>45540.700308194442</v>
       </c>
@@ -1498,7 +1503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:49" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>45540.71178445602</v>
       </c>
@@ -1647,7 +1652,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:49" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>45540.756249270838</v>
       </c>
@@ -1793,7 +1798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:49" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>45540.783696712962</v>
       </c>
@@ -1942,7 +1947,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:49" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>45540.802029571758</v>
       </c>
@@ -2088,7 +2093,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:49" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>45540.80520412037</v>
       </c>
@@ -2237,7 +2242,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:49" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>45540.838762314816</v>
       </c>
@@ -2383,7 +2388,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:49" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>45540.894243356481</v>
       </c>
@@ -2529,7 +2534,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:49" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>45540.987715162039</v>
       </c>
@@ -2678,7 +2683,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:49" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>45541.127554351857</v>
       </c>
@@ -2824,7 +2829,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:49" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>45541.41719015046</v>
       </c>
@@ -2970,7 +2975,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:49" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>45541.508837534726</v>
       </c>
@@ -3116,7 +3121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:49" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>45543.767461458337</v>
       </c>
@@ -3262,7 +3267,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:49" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>45544.549161099538</v>
       </c>
@@ -3408,7 +3413,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:49" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>45547.528488495373</v>
       </c>
@@ -3706,7 +3711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:49" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>45547.772497928236</v>
       </c>
@@ -3852,7 +3857,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:49" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>45547.814017349534</v>
       </c>
@@ -3998,7 +4003,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:49" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>45548.333912476854</v>
       </c>
@@ -4144,7 +4149,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:49" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>45550.06369012731</v>
       </c>
@@ -4434,6 +4439,155 @@
       </c>
       <c r="AW26" s="1">
         <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="10">
+        <v>45552.581391539352</v>
+      </c>
+      <c r="B27" s="9">
+        <v>5</v>
+      </c>
+      <c r="C27" s="9">
+        <v>3</v>
+      </c>
+      <c r="D27" s="9">
+        <v>4</v>
+      </c>
+      <c r="E27" s="9">
+        <v>2</v>
+      </c>
+      <c r="F27" s="9">
+        <v>4</v>
+      </c>
+      <c r="G27" s="9">
+        <v>2</v>
+      </c>
+      <c r="H27" s="9">
+        <v>3</v>
+      </c>
+      <c r="I27" s="9">
+        <v>1</v>
+      </c>
+      <c r="J27" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="K27" s="9">
+        <v>4</v>
+      </c>
+      <c r="L27" s="9">
+        <v>4</v>
+      </c>
+      <c r="M27" s="9">
+        <v>1</v>
+      </c>
+      <c r="N27" s="9">
+        <v>1</v>
+      </c>
+      <c r="O27" s="9">
+        <v>4</v>
+      </c>
+      <c r="P27" s="9">
+        <v>4</v>
+      </c>
+      <c r="Q27" s="9">
+        <v>3</v>
+      </c>
+      <c r="R27" s="9">
+        <v>3</v>
+      </c>
+      <c r="S27" s="9">
+        <v>1</v>
+      </c>
+      <c r="T27" s="9">
+        <v>3</v>
+      </c>
+      <c r="U27" s="9">
+        <v>3</v>
+      </c>
+      <c r="V27" s="9">
+        <v>1</v>
+      </c>
+      <c r="W27" s="9">
+        <v>2</v>
+      </c>
+      <c r="X27" s="9">
+        <v>4</v>
+      </c>
+      <c r="Y27" s="9">
+        <v>1</v>
+      </c>
+      <c r="Z27" s="9">
+        <v>5</v>
+      </c>
+      <c r="AA27" s="9">
+        <v>1</v>
+      </c>
+      <c r="AB27" s="9">
+        <v>1</v>
+      </c>
+      <c r="AC27" s="9">
+        <v>3</v>
+      </c>
+      <c r="AD27" s="9">
+        <v>4</v>
+      </c>
+      <c r="AE27" s="9">
+        <v>1</v>
+      </c>
+      <c r="AF27" s="9">
+        <v>2</v>
+      </c>
+      <c r="AG27" s="9">
+        <v>1</v>
+      </c>
+      <c r="AH27" s="9">
+        <v>2</v>
+      </c>
+      <c r="AI27" s="9">
+        <v>3</v>
+      </c>
+      <c r="AJ27" s="9">
+        <v>3</v>
+      </c>
+      <c r="AK27" s="9">
+        <v>1</v>
+      </c>
+      <c r="AL27" s="9">
+        <v>1</v>
+      </c>
+      <c r="AM27" s="9">
+        <v>4</v>
+      </c>
+      <c r="AN27" s="9">
+        <v>3</v>
+      </c>
+      <c r="AO27" s="9">
+        <v>3</v>
+      </c>
+      <c r="AP27" s="9">
+        <v>1</v>
+      </c>
+      <c r="AQ27" s="9">
+        <v>1</v>
+      </c>
+      <c r="AR27" s="9">
+        <v>2</v>
+      </c>
+      <c r="AS27" s="9">
+        <v>1</v>
+      </c>
+      <c r="AT27" s="9">
+        <v>1</v>
+      </c>
+      <c r="AU27" s="9">
+        <v>5</v>
+      </c>
+      <c r="AV27" s="9">
+        <v>4</v>
+      </c>
+      <c r="AW27" s="9">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>